<commit_message>
new added data and sankey
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Final_Parameters/3i Infotech Ltd_Cleaned_Data.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Final_Parameters/3i Infotech Ltd_Cleaned_Data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="219">
   <si>
     <t>Balance Sheet of 3i Infotech(in Rs. Cr.)</t>
   </si>
@@ -362,6 +362,9 @@
     <t>P/l before exceptional items &amp; tax</t>
   </si>
   <si>
+    <t>Exceptional items</t>
+  </si>
+  <si>
     <t>P/l before tax</t>
   </si>
   <si>
@@ -540,6 +543,9 @@
   </si>
   <si>
     <t>P/L Before Exceptional Items &amp; Tax</t>
+  </si>
+  <si>
+    <t>Exceptional Items</t>
   </si>
   <si>
     <t>P/L Before Tax</t>
@@ -4101,13 +4107,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T47"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -4168,19 +4174,22 @@
       <c r="T1" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>109</v>
@@ -4189,51 +4198,54 @@
         <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H2" t="s">
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J2" t="s">
         <v>112</v>
       </c>
       <c r="K2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="L2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="N2" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="O2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="P2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="R2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="S2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="T2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>182</v>
+      </c>
+      <c r="U2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>90.95</v>
@@ -4265,23 +4277,20 @@
       <c r="K3">
         <v>-139.21</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>-139.21</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.23</v>
-      </c>
-      <c r="N3">
-        <v>-139.44</v>
       </c>
       <c r="O3">
         <v>-139.44</v>
       </c>
       <c r="P3">
+        <v>-139.44</v>
+      </c>
+      <c r="Q3">
         <v>571.9400000000001</v>
-      </c>
-      <c r="Q3">
-        <v>-2.52</v>
       </c>
       <c r="R3">
         <v>-2.52</v>
@@ -4292,10 +4301,13 @@
       <c r="T3">
         <v>-2.52</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3">
+        <v>-2.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>78.26000000000001</v>
@@ -4327,23 +4339,20 @@
       <c r="K4">
         <v>-95.98</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>-95.98</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1.5</v>
-      </c>
-      <c r="N4">
-        <v>-97.48</v>
       </c>
       <c r="O4">
         <v>-97.48</v>
       </c>
       <c r="P4">
+        <v>-97.48</v>
+      </c>
+      <c r="Q4">
         <v>571.9400000000001</v>
-      </c>
-      <c r="Q4">
-        <v>-1.79</v>
       </c>
       <c r="R4">
         <v>-1.79</v>
@@ -4354,10 +4363,13 @@
       <c r="T4">
         <v>-1.79</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4">
+        <v>-1.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>108.29</v>
@@ -4389,20 +4401,17 @@
       <c r="K5">
         <v>-100.4</v>
       </c>
-      <c r="L5">
-        <v>-100.4</v>
-      </c>
-      <c r="N5">
+      <c r="M5">
         <v>-100.4</v>
       </c>
       <c r="O5">
         <v>-100.4</v>
       </c>
       <c r="P5">
+        <v>-100.4</v>
+      </c>
+      <c r="Q5">
         <v>580.6799999999999</v>
-      </c>
-      <c r="Q5">
-        <v>-1.82</v>
       </c>
       <c r="R5">
         <v>-1.82</v>
@@ -4413,10 +4422,13 @@
       <c r="T5">
         <v>-1.82</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5">
+        <v>-1.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>93.17</v>
@@ -4448,20 +4460,17 @@
       <c r="K6">
         <v>-105.21</v>
       </c>
-      <c r="L6">
-        <v>-105.21</v>
-      </c>
-      <c r="N6">
+      <c r="M6">
         <v>-105.21</v>
       </c>
       <c r="O6">
         <v>-105.21</v>
       </c>
       <c r="P6">
+        <v>-105.21</v>
+      </c>
+      <c r="Q6">
         <v>576.34</v>
-      </c>
-      <c r="Q6">
-        <v>-1.92</v>
       </c>
       <c r="R6">
         <v>-1.92</v>
@@ -4472,10 +4481,13 @@
       <c r="T6">
         <v>-1.92</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6">
+        <v>-1.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7">
         <v>79.08</v>
@@ -4508,36 +4520,39 @@
         <v>-100.76</v>
       </c>
       <c r="L7">
+        <v>-35.85</v>
+      </c>
+      <c r="M7">
         <v>-136.61</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>-15.28</v>
-      </c>
-      <c r="N7">
-        <v>-121.33</v>
       </c>
       <c r="O7">
         <v>-121.33</v>
       </c>
       <c r="P7">
+        <v>-121.33</v>
+      </c>
+      <c r="Q7">
         <v>572.64</v>
-      </c>
-      <c r="Q7">
-        <v>-1.58</v>
       </c>
       <c r="R7">
         <v>-1.58</v>
       </c>
       <c r="S7">
-        <v>-2.2</v>
+        <v>-1.58</v>
       </c>
       <c r="T7">
         <v>-2.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7">
+        <v>-2.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8">
         <v>105.8</v>
@@ -4570,36 +4585,39 @@
         <v>-119.37</v>
       </c>
       <c r="L8">
+        <v>-329.79</v>
+      </c>
+      <c r="M8">
         <v>-449.16</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>2.02</v>
-      </c>
-      <c r="N8">
-        <v>-451.18</v>
       </c>
       <c r="O8">
         <v>-451.18</v>
       </c>
       <c r="P8">
+        <v>-451.18</v>
+      </c>
+      <c r="Q8">
         <v>586.12</v>
-      </c>
-      <c r="Q8">
-        <v>-2.17</v>
       </c>
       <c r="R8">
         <v>-2.17</v>
       </c>
       <c r="S8">
-        <v>-7.84</v>
+        <v>-2.17</v>
       </c>
       <c r="T8">
         <v>-7.84</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8">
+        <v>-7.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B9">
         <v>79.54000000000001</v>
@@ -4631,20 +4649,17 @@
       <c r="K9">
         <v>-17.65</v>
       </c>
-      <c r="L9">
-        <v>-17.65</v>
-      </c>
-      <c r="N9">
+      <c r="M9">
         <v>-17.65</v>
       </c>
       <c r="O9">
         <v>-17.65</v>
       </c>
       <c r="P9">
+        <v>-17.65</v>
+      </c>
+      <c r="Q9">
         <v>636.1900000000001</v>
-      </c>
-      <c r="Q9">
-        <v>-0.36</v>
       </c>
       <c r="R9">
         <v>-0.36</v>
@@ -4655,10 +4670,13 @@
       <c r="T9">
         <v>-0.36</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10">
         <v>84.08</v>
@@ -4690,20 +4708,17 @@
       <c r="K10">
         <v>-111.91</v>
       </c>
-      <c r="L10">
-        <v>-111.91</v>
-      </c>
-      <c r="N10">
+      <c r="M10">
         <v>-111.91</v>
       </c>
       <c r="O10">
         <v>-111.91</v>
       </c>
       <c r="P10">
+        <v>-111.91</v>
+      </c>
+      <c r="Q10">
         <v>612.52</v>
-      </c>
-      <c r="Q10">
-        <v>-1.91</v>
       </c>
       <c r="R10">
         <v>-1.91</v>
@@ -4714,10 +4729,13 @@
       <c r="T10">
         <v>-1.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10">
+        <v>-1.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B11">
         <v>81.77</v>
@@ -4749,20 +4767,17 @@
       <c r="K11">
         <v>-101.52</v>
       </c>
-      <c r="L11">
-        <v>-101.52</v>
-      </c>
-      <c r="N11">
+      <c r="M11">
         <v>-101.52</v>
       </c>
       <c r="O11">
         <v>-101.52</v>
       </c>
       <c r="P11">
+        <v>-101.52</v>
+      </c>
+      <c r="Q11">
         <v>612.4299999999999</v>
-      </c>
-      <c r="Q11">
-        <v>-1.75</v>
       </c>
       <c r="R11">
         <v>-1.75</v>
@@ -4773,10 +4788,13 @@
       <c r="T11">
         <v>-1.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B12">
         <v>93.45999999999999</v>
@@ -4809,36 +4827,39 @@
         <v>-18.6</v>
       </c>
       <c r="L12">
+        <v>-360.82</v>
+      </c>
+      <c r="M12">
         <v>-379.42</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>21.54</v>
-      </c>
-      <c r="N12">
-        <v>-400.96</v>
       </c>
       <c r="O12">
         <v>-400.96</v>
       </c>
       <c r="P12">
+        <v>-400.96</v>
+      </c>
+      <c r="Q12">
         <v>603.75</v>
-      </c>
-      <c r="Q12">
-        <v>-0.76</v>
       </c>
       <c r="R12">
         <v>-0.76</v>
       </c>
       <c r="S12">
-        <v>-6.84</v>
+        <v>-0.76</v>
       </c>
       <c r="T12">
         <v>-6.84</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12">
+        <v>-6.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B13">
         <v>64.56999999999999</v>
@@ -4870,20 +4891,17 @@
       <c r="K13">
         <v>56.79</v>
       </c>
-      <c r="L13">
-        <v>56.79</v>
-      </c>
-      <c r="N13">
+      <c r="M13">
         <v>56.79</v>
       </c>
       <c r="O13">
         <v>56.79</v>
       </c>
       <c r="P13">
+        <v>56.79</v>
+      </c>
+      <c r="Q13">
         <v>1047.45</v>
-      </c>
-      <c r="Q13">
-        <v>0.52</v>
       </c>
       <c r="R13">
         <v>0.52</v>
@@ -4894,10 +4912,13 @@
       <c r="T13">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B14">
         <v>55.93</v>
@@ -4929,37 +4950,37 @@
       <c r="K14">
         <v>14.44</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>14.44</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.19</v>
-      </c>
-      <c r="N14">
-        <v>14.25</v>
       </c>
       <c r="O14">
         <v>14.25</v>
       </c>
       <c r="P14">
+        <v>14.25</v>
+      </c>
+      <c r="Q14">
         <v>898.88</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.3</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>0.15</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>0.3</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>0.15</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15">
         <v>81.33</v>
@@ -4991,20 +5012,17 @@
       <c r="K15">
         <v>15.51</v>
       </c>
-      <c r="L15">
-        <v>15.51</v>
-      </c>
-      <c r="N15">
+      <c r="M15">
         <v>15.51</v>
       </c>
       <c r="O15">
         <v>15.51</v>
       </c>
       <c r="P15">
+        <v>15.51</v>
+      </c>
+      <c r="Q15">
         <v>640.8</v>
-      </c>
-      <c r="Q15">
-        <v>0.24</v>
       </c>
       <c r="R15">
         <v>0.24</v>
@@ -5015,10 +5033,13 @@
       <c r="T15">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B16">
         <v>84.84999999999999</v>
@@ -5051,22 +5072,22 @@
         <v>-7.4</v>
       </c>
       <c r="L16">
+        <v>-698.03</v>
+      </c>
+      <c r="M16">
         <v>-705.4299999999999</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>127.15</v>
-      </c>
-      <c r="N16">
-        <v>-832.58</v>
       </c>
       <c r="O16">
         <v>-832.58</v>
       </c>
       <c r="P16">
+        <v>-832.58</v>
+      </c>
+      <c r="Q16">
         <v>640.8</v>
-      </c>
-      <c r="Q16">
-        <v>-2.1</v>
       </c>
       <c r="R16">
         <v>-2.1</v>
@@ -5077,10 +5098,13 @@
       <c r="T16">
         <v>-2.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B17">
         <v>66.98999999999999</v>
@@ -5113,22 +5137,22 @@
         <v>29.95</v>
       </c>
       <c r="L17">
+        <v>-25.6</v>
+      </c>
+      <c r="M17">
         <v>4.35</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>-1.37</v>
-      </c>
-      <c r="N17">
-        <v>5.72</v>
       </c>
       <c r="O17">
         <v>5.72</v>
       </c>
       <c r="P17">
+        <v>5.72</v>
+      </c>
+      <c r="Q17">
         <v>1183.65</v>
-      </c>
-      <c r="Q17">
-        <v>0.05</v>
       </c>
       <c r="R17">
         <v>0.05</v>
@@ -5139,10 +5163,13 @@
       <c r="T17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="U17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18">
         <v>58.12</v>
@@ -5175,19 +5202,19 @@
         <v>20.35</v>
       </c>
       <c r="L18">
+        <v>-18.4</v>
+      </c>
+      <c r="M18">
         <v>1.95</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>1.95</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>-2.1</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>1334.15</v>
-      </c>
-      <c r="Q18">
-        <v>-0.02</v>
       </c>
       <c r="R18">
         <v>-0.02</v>
@@ -5198,10 +5225,13 @@
       <c r="T18">
         <v>-0.02</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="U18">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B19">
         <v>57.72</v>
@@ -5234,19 +5264,19 @@
         <v>-138.21</v>
       </c>
       <c r="L19">
+        <v>12.22</v>
+      </c>
+      <c r="M19">
         <v>-125.99</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>-125.99</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>-130.09</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>1333.09</v>
-      </c>
-      <c r="Q19">
-        <v>-0.99</v>
       </c>
       <c r="R19">
         <v>-0.99</v>
@@ -5257,10 +5287,13 @@
       <c r="T19">
         <v>-0.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="U19">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20">
         <v>55.38</v>
@@ -5293,19 +5326,19 @@
         <v>18.76</v>
       </c>
       <c r="L20">
+        <v>-3.05</v>
+      </c>
+      <c r="M20">
         <v>15.71</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>15.71</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>17.7</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>1286</v>
-      </c>
-      <c r="Q20">
-        <v>0.14</v>
       </c>
       <c r="R20">
         <v>0.14</v>
@@ -5316,10 +5349,13 @@
       <c r="T20">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="U20">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B21">
         <v>58.7</v>
@@ -5352,19 +5388,19 @@
         <v>3.76</v>
       </c>
       <c r="L21">
+        <v>40.47</v>
+      </c>
+      <c r="M21">
         <v>44.23</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>44.23</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>39.54</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>1615.55</v>
-      </c>
-      <c r="Q21">
-        <v>0.24</v>
       </c>
       <c r="R21">
         <v>0.24</v>
@@ -5375,10 +5411,13 @@
       <c r="T21">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="U21">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B22">
         <v>66.29000000000001</v>
@@ -5411,19 +5450,19 @@
         <v>14.85</v>
       </c>
       <c r="L22">
+        <v>17.35</v>
+      </c>
+      <c r="M22">
         <v>32.2</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>32.2</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>27.75</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>1615.36</v>
-      </c>
-      <c r="Q22">
-        <v>0.17</v>
       </c>
       <c r="R22">
         <v>0.17</v>
@@ -5434,10 +5473,13 @@
       <c r="T22">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="U22">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B23">
         <v>74.27</v>
@@ -5470,19 +5512,19 @@
         <v>152.5</v>
       </c>
       <c r="L23">
+        <v>-37.76</v>
+      </c>
+      <c r="M23">
         <v>114.74</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>114.74</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>110.25</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>1616.64</v>
-      </c>
-      <c r="Q23">
-        <v>0.68</v>
       </c>
       <c r="R23">
         <v>0.68</v>
@@ -5493,10 +5535,13 @@
       <c r="T23">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="U23">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B24">
         <v>75.67</v>
@@ -5529,19 +5574,19 @@
         <v>30.46</v>
       </c>
       <c r="L24">
+        <v>52.69</v>
+      </c>
+      <c r="M24">
         <v>83.15000000000001</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>83.15000000000001</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>78.61</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>1615.91</v>
-      </c>
-      <c r="Q24">
-        <v>0.49</v>
       </c>
       <c r="R24">
         <v>0.49</v>
@@ -5552,10 +5597,13 @@
       <c r="T24">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="U24">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B25">
         <v>80.98</v>
@@ -5588,19 +5636,19 @@
         <v>17.72</v>
       </c>
       <c r="L25">
+        <v>15.75</v>
+      </c>
+      <c r="M25">
         <v>33.47</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>33.47</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>28.16</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>1616.64</v>
-      </c>
-      <c r="Q25">
-        <v>0.17</v>
       </c>
       <c r="R25">
         <v>0.17</v>
@@ -5611,10 +5659,13 @@
       <c r="T25">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="U25">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26">
         <v>74.20999999999999</v>
@@ -5647,19 +5698,19 @@
         <v>9.199999999999999</v>
       </c>
       <c r="L26">
+        <v>-5.85</v>
+      </c>
+      <c r="M26">
         <v>3.35</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>3.35</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>-2.03</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>1616.64</v>
-      </c>
-      <c r="Q26">
-        <v>-0.01</v>
       </c>
       <c r="R26">
         <v>-0.01</v>
@@ -5670,10 +5721,13 @@
       <c r="T26">
         <v>-0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="U26">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B27">
         <v>75.28</v>
@@ -5706,19 +5760,19 @@
         <v>30.77</v>
       </c>
       <c r="L27">
+        <v>-3.72</v>
+      </c>
+      <c r="M27">
         <v>27.05</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>27.05</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>22.5</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>1616.64</v>
-      </c>
-      <c r="Q27">
-        <v>0.14</v>
       </c>
       <c r="R27">
         <v>0.14</v>
@@ -5729,10 +5783,13 @@
       <c r="T27">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="U27">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28">
         <v>91.59999999999999</v>
@@ -5765,33 +5822,36 @@
         <v>19.72</v>
       </c>
       <c r="L28">
-        <v>30</v>
-      </c>
-      <c r="N28">
+        <v>10.28</v>
+      </c>
+      <c r="M28">
         <v>30</v>
       </c>
       <c r="O28">
         <v>30</v>
       </c>
       <c r="P28">
+        <v>30</v>
+      </c>
+      <c r="Q28">
         <v>1616.64</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>0.19</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>0.22</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>0.19</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>0.22</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B29">
         <v>86.72</v>
@@ -5824,22 +5884,22 @@
         <v>27.92</v>
       </c>
       <c r="L29">
+        <v>-8.15</v>
+      </c>
+      <c r="M29">
         <v>19.77</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>-0.12</v>
-      </c>
-      <c r="N29">
-        <v>19.89</v>
       </c>
       <c r="O29">
         <v>19.89</v>
       </c>
       <c r="P29">
+        <v>19.89</v>
+      </c>
+      <c r="Q29">
         <v>1616.65</v>
-      </c>
-      <c r="Q29">
-        <v>0.16</v>
       </c>
       <c r="R29">
         <v>0.16</v>
@@ -5850,10 +5910,13 @@
       <c r="T29">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="U29">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B30">
         <v>86.33</v>
@@ -5886,22 +5949,22 @@
         <v>8.44</v>
       </c>
       <c r="L30">
+        <v>-5.67</v>
+      </c>
+      <c r="M30">
         <v>2.77</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>0.19</v>
-      </c>
-      <c r="N30">
-        <v>2.58</v>
       </c>
       <c r="O30">
         <v>2.58</v>
       </c>
       <c r="P30">
+        <v>2.58</v>
+      </c>
+      <c r="Q30">
         <v>1616.65</v>
-      </c>
-      <c r="Q30">
-        <v>0.05</v>
       </c>
       <c r="R30">
         <v>0.05</v>
@@ -5912,10 +5975,13 @@
       <c r="T30">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="U30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B31">
         <v>81.58</v>
@@ -5948,22 +6014,22 @@
         <v>29.85</v>
       </c>
       <c r="L31">
+        <v>-5.75</v>
+      </c>
+      <c r="M31">
         <v>24.1</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>0.06</v>
-      </c>
-      <c r="N31">
-        <v>24.04</v>
       </c>
       <c r="O31">
         <v>24.04</v>
       </c>
       <c r="P31">
+        <v>24.04</v>
+      </c>
+      <c r="Q31">
         <v>1616.65</v>
-      </c>
-      <c r="Q31">
-        <v>0.18</v>
       </c>
       <c r="R31">
         <v>0.18</v>
@@ -5974,10 +6040,13 @@
       <c r="T31">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="U31">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B32">
         <v>91.48</v>
@@ -6010,22 +6079,22 @@
         <v>77.23999999999999</v>
       </c>
       <c r="L32">
+        <v>-5.41</v>
+      </c>
+      <c r="M32">
         <v>71.83</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>0.07000000000000001</v>
-      </c>
-      <c r="N32">
-        <v>71.76000000000001</v>
       </c>
       <c r="O32">
         <v>71.76000000000001</v>
       </c>
       <c r="P32">
+        <v>71.76000000000001</v>
+      </c>
+      <c r="Q32">
         <v>1616.65</v>
-      </c>
-      <c r="Q32">
-        <v>0.48</v>
       </c>
       <c r="R32">
         <v>0.48</v>
@@ -6036,10 +6105,13 @@
       <c r="T32">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="U32">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B33">
         <v>46.86</v>
@@ -6072,19 +6144,19 @@
         <v>-13.16</v>
       </c>
       <c r="L33">
-        <v>-21.77</v>
-      </c>
-      <c r="N33">
+        <v>-8.609999999999999</v>
+      </c>
+      <c r="M33">
         <v>-21.77</v>
       </c>
       <c r="O33">
         <v>-21.77</v>
       </c>
       <c r="P33">
+        <v>-21.77</v>
+      </c>
+      <c r="Q33">
         <v>165.44</v>
-      </c>
-      <c r="Q33">
-        <v>-1.32</v>
       </c>
       <c r="R33">
         <v>-1.32</v>
@@ -6095,10 +6167,13 @@
       <c r="T33">
         <v>-1.32</v>
       </c>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="U33">
+        <v>-1.32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B34">
         <v>58.63</v>
@@ -6131,19 +6206,19 @@
         <v>-15.67</v>
       </c>
       <c r="L34">
-        <v>-12.42</v>
-      </c>
-      <c r="N34">
+        <v>3.25</v>
+      </c>
+      <c r="M34">
         <v>-12.42</v>
       </c>
       <c r="O34">
         <v>-12.42</v>
       </c>
       <c r="P34">
+        <v>-12.42</v>
+      </c>
+      <c r="Q34">
         <v>161.67</v>
-      </c>
-      <c r="Q34">
-        <v>-0.77</v>
       </c>
       <c r="R34">
         <v>-0.77</v>
@@ -6154,10 +6229,13 @@
       <c r="T34">
         <v>-0.77</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="U34">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B35">
         <v>53.1</v>
@@ -6190,19 +6268,19 @@
         <v>7.65</v>
       </c>
       <c r="L35">
-        <v>21.75</v>
-      </c>
-      <c r="N35">
+        <v>14.1</v>
+      </c>
+      <c r="M35">
         <v>21.75</v>
       </c>
       <c r="O35">
         <v>21.75</v>
       </c>
       <c r="P35">
+        <v>21.75</v>
+      </c>
+      <c r="Q35">
         <v>1616.65</v>
-      </c>
-      <c r="Q35">
-        <v>0.11</v>
       </c>
       <c r="R35">
         <v>0.11</v>
@@ -6213,10 +6291,13 @@
       <c r="T35">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="U35">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B36">
         <v>52.22</v>
@@ -6249,22 +6330,22 @@
         <v>-35.85</v>
       </c>
       <c r="L36">
+        <v>290.51</v>
+      </c>
+      <c r="M36">
         <v>254.66</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>0.01</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>254.65</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>277.91</v>
       </c>
-      <c r="P36">
+      <c r="Q36">
         <v>1616.65</v>
-      </c>
-      <c r="Q36">
-        <v>1.61</v>
       </c>
       <c r="R36">
         <v>1.61</v>
@@ -6275,10 +6356,13 @@
       <c r="T36">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="U36">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37">
         <v>54.01</v>
@@ -6311,19 +6395,19 @@
         <v>3.93</v>
       </c>
       <c r="L37">
-        <v>20.86</v>
-      </c>
-      <c r="N37">
+        <v>16.93</v>
+      </c>
+      <c r="M37">
         <v>20.86</v>
       </c>
       <c r="O37">
         <v>20.86</v>
       </c>
       <c r="P37">
+        <v>20.86</v>
+      </c>
+      <c r="Q37">
         <v>167.94</v>
-      </c>
-      <c r="Q37">
-        <v>1.25</v>
       </c>
       <c r="R37">
         <v>1.25</v>
@@ -6334,10 +6418,13 @@
       <c r="T37">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="U37">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B38">
         <v>69.65000000000001</v>
@@ -6370,27 +6457,30 @@
         <v>18.41</v>
       </c>
       <c r="L38">
-        <v>41.5</v>
-      </c>
-      <c r="N38">
+        <v>23.09</v>
+      </c>
+      <c r="M38">
         <v>41.5</v>
       </c>
       <c r="O38">
         <v>41.5</v>
       </c>
       <c r="P38">
+        <v>41.5</v>
+      </c>
+      <c r="Q38">
         <v>168.39</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <v>2.46</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <v>2.46</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B39">
         <v>68.62</v>
@@ -6423,33 +6513,36 @@
         <v>14.52</v>
       </c>
       <c r="L39">
-        <v>6.77</v>
-      </c>
-      <c r="N39">
+        <v>-7.75</v>
+      </c>
+      <c r="M39">
         <v>6.77</v>
       </c>
       <c r="O39">
         <v>6.77</v>
       </c>
       <c r="P39">
+        <v>6.77</v>
+      </c>
+      <c r="Q39">
         <v>168.39</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>0.4</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <v>0.05</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <v>0.4</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B40">
         <v>62.58</v>
@@ -6481,20 +6574,17 @@
       <c r="K40">
         <v>25.54</v>
       </c>
-      <c r="L40">
-        <v>25.54</v>
-      </c>
-      <c r="N40">
+      <c r="M40">
         <v>25.54</v>
       </c>
       <c r="O40">
         <v>25.54</v>
       </c>
       <c r="P40">
+        <v>25.54</v>
+      </c>
+      <c r="Q40">
         <v>168.38</v>
-      </c>
-      <c r="Q40">
-        <v>1.52</v>
       </c>
       <c r="R40">
         <v>1.52</v>
@@ -6505,10 +6595,13 @@
       <c r="T40">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="41" spans="1:20">
+      <c r="U40">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B41">
         <v>82.78</v>
@@ -6541,19 +6634,19 @@
         <v>-12.4</v>
       </c>
       <c r="L41">
-        <v>-15.3</v>
-      </c>
-      <c r="N41">
+        <v>-2.9</v>
+      </c>
+      <c r="M41">
         <v>-15.3</v>
       </c>
       <c r="O41">
         <v>-15.3</v>
       </c>
       <c r="P41">
+        <v>-15.3</v>
+      </c>
+      <c r="Q41">
         <v>168.47</v>
-      </c>
-      <c r="Q41">
-        <v>-0.91</v>
       </c>
       <c r="R41">
         <v>-0.91</v>
@@ -6564,10 +6657,13 @@
       <c r="T41">
         <v>-0.91</v>
       </c>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="U41">
+        <v>-0.91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B42">
         <v>75.40000000000001</v>
@@ -6600,19 +6696,19 @@
         <v>-20.7</v>
       </c>
       <c r="L42">
-        <v>-21.56</v>
-      </c>
-      <c r="N42">
+        <v>-0.86</v>
+      </c>
+      <c r="M42">
         <v>-21.56</v>
       </c>
       <c r="O42">
         <v>-21.56</v>
       </c>
       <c r="P42">
+        <v>-21.56</v>
+      </c>
+      <c r="Q42">
         <v>168.47</v>
-      </c>
-      <c r="Q42">
-        <v>-1.28</v>
       </c>
       <c r="R42">
         <v>-1.28</v>
@@ -6623,10 +6719,13 @@
       <c r="T42">
         <v>-1.28</v>
       </c>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="U42">
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B43">
         <v>91.64</v>
@@ -6659,19 +6758,19 @@
         <v>-221.21</v>
       </c>
       <c r="L43">
-        <v>-642.91</v>
-      </c>
-      <c r="N43">
+        <v>-421.7</v>
+      </c>
+      <c r="M43">
         <v>-642.91</v>
       </c>
       <c r="O43">
         <v>-642.91</v>
       </c>
       <c r="P43">
+        <v>-642.91</v>
+      </c>
+      <c r="Q43">
         <v>168.77</v>
-      </c>
-      <c r="Q43">
-        <v>-38.1</v>
       </c>
       <c r="R43">
         <v>-38.1</v>
@@ -6682,10 +6781,13 @@
       <c r="T43">
         <v>-38.1</v>
       </c>
-    </row>
-    <row r="44" spans="1:20">
+      <c r="U43">
+        <v>-38.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B44">
         <v>91.06999999999999</v>
@@ -6717,34 +6819,34 @@
       <c r="K44">
         <v>-114.78</v>
       </c>
-      <c r="L44">
-        <v>-114.78</v>
-      </c>
-      <c r="N44">
+      <c r="M44">
         <v>-114.78</v>
       </c>
       <c r="O44">
         <v>-114.78</v>
       </c>
       <c r="P44">
+        <v>-114.78</v>
+      </c>
+      <c r="Q44">
         <v>168.64</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>-6.81</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <v>-6.78</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>-6.81</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>-6.78</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B45">
         <v>89.40000000000001</v>
@@ -6776,34 +6878,34 @@
       <c r="K45">
         <v>13.53</v>
       </c>
-      <c r="L45">
-        <v>13.53</v>
-      </c>
-      <c r="N45">
+      <c r="M45">
         <v>13.53</v>
       </c>
       <c r="O45">
         <v>13.53</v>
       </c>
       <c r="P45">
+        <v>13.53</v>
+      </c>
+      <c r="Q45">
         <v>169.4</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <v>0.8</v>
       </c>
-      <c r="R45">
+      <c r="S45">
         <v>0.79</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>0.8</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>0.79</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B46">
         <v>89.77</v>
@@ -6835,20 +6937,17 @@
       <c r="K46">
         <v>-9</v>
       </c>
-      <c r="L46">
-        <v>-9</v>
-      </c>
-      <c r="N46">
+      <c r="M46">
         <v>-9</v>
       </c>
       <c r="O46">
         <v>-9</v>
       </c>
       <c r="P46">
+        <v>-9</v>
+      </c>
+      <c r="Q46">
         <v>169.24</v>
-      </c>
-      <c r="Q46">
-        <v>-0.53</v>
       </c>
       <c r="R46">
         <v>-0.53</v>
@@ -6859,10 +6958,13 @@
       <c r="T46">
         <v>-0.53</v>
       </c>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="U46">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B47">
         <v>91.83</v>
@@ -6895,19 +6997,19 @@
         <v>-49.87</v>
       </c>
       <c r="L47">
-        <v>-45.64</v>
-      </c>
-      <c r="N47">
+        <v>4.23</v>
+      </c>
+      <c r="M47">
         <v>-45.64</v>
       </c>
       <c r="O47">
         <v>-45.64</v>
       </c>
       <c r="P47">
+        <v>-45.64</v>
+      </c>
+      <c r="Q47">
         <v>169.23</v>
-      </c>
-      <c r="Q47">
-        <v>-2.7</v>
       </c>
       <c r="R47">
         <v>-2.7</v>
@@ -6916,6 +7018,9 @@
         <v>-2.7</v>
       </c>
       <c r="T47">
+        <v>-2.7</v>
+      </c>
+      <c r="U47">
         <v>-2.7</v>
       </c>
     </row>
@@ -6934,114 +7039,114 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="J2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="K2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="L2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="N2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="O2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="P2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Q2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="R2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:18">

</xml_diff>